<commit_message>
add few more test cases
</commit_message>
<xml_diff>
--- a/MercuryToursFrameworkDemo/resources/MasterData.xlsx
+++ b/MercuryToursFrameworkDemo/resources/MasterData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Shweta\workspace\Selenium\MercuryToursFrameworkDemo\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shweta\Documents\GitHub\Selenium_Work\MercuryToursFrameworkDemo\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="39">
   <si>
     <t>Hello World!!!</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Username</t>
   </si>
   <si>
-    <t>testpwd5</t>
-  </si>
-  <si>
-    <t>testuser5</t>
-  </si>
-  <si>
     <t>testLoginSuccessful</t>
   </si>
   <si>
@@ -88,6 +82,66 @@
   </si>
   <si>
     <t>Portland</t>
+  </si>
+  <si>
+    <t>testLoginUnSuccessful</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>cdf</t>
+  </si>
+  <si>
+    <t>tutorial2</t>
+  </si>
+  <si>
+    <t>tutorial3</t>
+  </si>
+  <si>
+    <t>testSignOff</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>testDepartDate</t>
+  </si>
+  <si>
+    <t>departDate</t>
+  </si>
+  <si>
+    <t>DepartMonth</t>
+  </si>
+  <si>
+    <t>returnDate</t>
+  </si>
+  <si>
+    <t>returnMonth</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>testReturnDate</t>
+  </si>
+  <si>
+    <t>testReturnToDepartCity</t>
+  </si>
+  <si>
+    <t>testDepartToReturnCity</t>
   </si>
 </sst>
 </file>
@@ -137,11 +191,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A30" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,9 +488,9 @@
     <col min="1" max="1" width="45.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -444,42 +499,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -487,94 +542,602 @@
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="F38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
         <v>13</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F39" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>